<commit_message>
removing rowId, isHeader. Started adding column codes
</commit_message>
<xml_diff>
--- a/com.kaleidoscope.core.aux.simpleexcel/Resources/Relationship.xlsx
+++ b/com.kaleidoscope.core.aux.simpleexcel/Resources/Relationship.xlsx
@@ -7,14 +7,14 @@
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="RelationShip" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Components</t>
   </si>
@@ -26,6 +26,9 @@
   </si>
   <si>
     <t>Review</t>
+  </si>
+  <si>
+    <t>org.emoflon.ibex.tgg.core.language</t>
   </si>
 </sst>
 </file>
@@ -49,12 +52,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -69,9 +78,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -376,10 +386,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -403,6 +413,14 @@
         <v>3</v>
       </c>
     </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
committing. Date : 04.02.2018
</commit_message>
<xml_diff>
--- a/com.kaleidoscope.core.aux.simpleexcel/Resources/Relationship.xlsx
+++ b/com.kaleidoscope.core.aux.simpleexcel/Resources/Relationship.xlsx
@@ -7,14 +7,14 @@
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="RelationShip" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Components</t>
   </si>
@@ -29,6 +29,18 @@
   </si>
   <si>
     <t>org.emoflon.ibex.tgg.core.language</t>
+  </si>
+  <si>
+    <t>org.emoflon.ibex.tgg.core.runtime</t>
+  </si>
+  <si>
+    <t>(org.emoflon.ibex.tgg.ide).IbexTGGBuilderExtension</t>
+  </si>
+  <si>
+    <t>(org.emoflon.ibex.tgg.ide).IbexTGGBuilderExtension_1</t>
+  </si>
+  <si>
+    <t>(org.emoflon.ibex.tgg.ide).IbexTGGBuilderExtension_2</t>
   </si>
 </sst>
 </file>
@@ -52,16 +64,34 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -78,10 +108,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -386,10 +419,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -400,26 +433,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="2"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="1"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>